<commit_message>
Se ha añadido fusibles i cables 5
</commit_message>
<xml_diff>
--- a/Excels/cables.xlsx
+++ b/Excels/cables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\comunidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F955C487-A4CE-411E-BDC7-A10E0FB5E4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD04694-B47B-4C70-A4F1-FE1C6CB49C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="cables" sheetId="1" r:id="rId1"/>
+    <sheet name="fusibles" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>area (mm^2)</t>
   </si>
@@ -62,6 +63,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Fusibles (A)</t>
   </si>
 </sst>
 </file>
@@ -1019,11 +1023,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFECFDA0-9020-4EC9-B649-3A07705A7D2A}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E04ABD9-E41A-4333-B922-8C07DE8DB164}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se ha modificado el excel "cables" 1
</commit_message>
<xml_diff>
--- a/Excels/cables.xlsx
+++ b/Excels/cables.xlsx
@@ -568,8 +568,8 @@
       <c r="A7" s="1">
         <v>40.0</v>
       </c>
-      <c r="B7" s="1">
-        <v>15.0</v>
+      <c r="B7" s="2">
+        <v>16.0</v>
       </c>
       <c r="C7" s="1">
         <v>45.0</v>

</xml_diff>

<commit_message>
Se ha actualizado el excel "cables"
</commit_message>
<xml_diff>
--- a/Excels/cables.xlsx
+++ b/Excels/cables.xlsx
@@ -4,23 +4,21 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="cables" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="fusibles" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="termic" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="fusibles" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="pPHTVzD6dwxJVbFZxrE7G5q36Mg22jtT5rXL4RIiApY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="mZoLPUkbsq35IJ7wFjA9HB1Rwez6c3zF9Tk4CmKrDF4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
-  <si>
-    <t>Termic (A)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>area (mm^2)</t>
   </si>
@@ -32,6 +30,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Termic (A)</t>
   </si>
   <si>
     <t>Fusibles (A)</t>
@@ -89,6 +90,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -304,640 +309,595 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6.0</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="M1" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="J1" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="L1" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="M1" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="N1" s="1">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>16.5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="C3" s="1">
         <v>16.0</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>15.0</v>
-      </c>
       <c r="D3" s="1">
-        <v>16.0</v>
+        <v>17.5</v>
       </c>
       <c r="E3" s="1">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="F3" s="1">
-        <v>18.5</v>
+        <v>21.0</v>
       </c>
       <c r="G3" s="1">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="H3" s="1">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="I3" s="1">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="J3" s="1">
-        <v>26.0</v>
+        <v>26.5</v>
       </c>
       <c r="K3" s="1">
-        <v>26.5</v>
+        <v>29.0</v>
       </c>
       <c r="L3" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="M3" s="1">
         <v>33.0</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>4</v>
+      <c r="M3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B4" s="1">
         <v>20.0</v>
       </c>
-      <c r="B4" s="1">
-        <v>4.0</v>
-      </c>
       <c r="C4" s="1">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="D4" s="1">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="E4" s="1">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="F4" s="1">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="G4" s="1">
-        <v>27.0</v>
+        <v>30.0</v>
       </c>
       <c r="H4" s="1">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="I4" s="1">
-        <v>31.0</v>
+        <v>34.0</v>
       </c>
       <c r="J4" s="1">
-        <v>34.0</v>
+        <v>36.0</v>
       </c>
       <c r="K4" s="1">
-        <v>36.0</v>
+        <v>38.0</v>
       </c>
       <c r="L4" s="1">
-        <v>38.0</v>
-      </c>
-      <c r="M4" s="1">
         <v>45.0</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>4</v>
+      <c r="M4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B5" s="1">
         <v>25.0</v>
       </c>
-      <c r="B5" s="1">
-        <v>6.0</v>
-      </c>
       <c r="C5" s="1">
-        <v>25.0</v>
+        <v>17.0</v>
       </c>
       <c r="D5" s="1">
-        <v>17.0</v>
+        <v>30.0</v>
       </c>
       <c r="E5" s="1">
-        <v>30.0</v>
+        <v>32.0</v>
       </c>
       <c r="F5" s="1">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
       <c r="G5" s="1">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="H5" s="1">
-        <v>37.0</v>
+        <v>40.0</v>
       </c>
       <c r="I5" s="1">
-        <v>40.0</v>
+        <v>44.0</v>
       </c>
       <c r="J5" s="1">
-        <v>44.0</v>
+        <v>48.0</v>
       </c>
       <c r="K5" s="1">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
       <c r="L5" s="1">
-        <v>49.0</v>
-      </c>
-      <c r="M5" s="1">
         <v>57.0</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>4</v>
+      <c r="M5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>32.0</v>
+        <v>10.0</v>
       </c>
       <c r="B6" s="1">
-        <v>10.0</v>
+        <v>34.0</v>
       </c>
       <c r="C6" s="1">
-        <v>34.0</v>
+        <v>37.0</v>
       </c>
       <c r="D6" s="1">
-        <v>37.0</v>
+        <v>40.0</v>
       </c>
       <c r="E6" s="1">
-        <v>40.0</v>
+        <v>44.0</v>
       </c>
       <c r="F6" s="1">
-        <v>44.0</v>
+        <v>50.0</v>
       </c>
       <c r="G6" s="1">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
       <c r="H6" s="1">
-        <v>52.0</v>
+        <v>54.0</v>
       </c>
       <c r="I6" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>68.0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>76.0</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="D7" s="1">
         <v>54.0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>65.0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>68.0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>76.0</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>40.0</v>
-      </c>
-      <c r="B7" s="2">
-        <v>16.0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45.0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>49.0</v>
       </c>
       <c r="E7" s="1">
         <v>54.0</v>
       </c>
       <c r="F7" s="1">
-        <v>54.0</v>
+        <v>66.0</v>
       </c>
       <c r="G7" s="1">
-        <v>66.0</v>
+        <v>70.0</v>
       </c>
       <c r="H7" s="1">
-        <v>70.0</v>
+        <v>73.0</v>
       </c>
       <c r="I7" s="1">
-        <v>73.0</v>
+        <v>81.0</v>
       </c>
       <c r="J7" s="1">
-        <v>81.0</v>
+        <v>87.0</v>
       </c>
       <c r="K7" s="1">
-        <v>87.0</v>
+        <v>91.0</v>
       </c>
       <c r="L7" s="1">
-        <v>91.0</v>
-      </c>
-      <c r="M7" s="1">
         <v>105.0</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>4</v>
+      <c r="M7" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>59.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>77.0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>84.0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>88.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>103.0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>110.0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>116.0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>123.0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>77.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>86.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>96.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>104.0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>110.0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>119.0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>127.0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>137.0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>144.0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>154.0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>174.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
         <v>50.0</v>
       </c>
-      <c r="B8" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>59.0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>64.0</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C10" s="1">
+        <v>94.0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>103.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>117.0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>125.0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>133.0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>145.0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>155.0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>167.0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>175.0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>168.0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>210.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
         <v>70.0</v>
       </c>
-      <c r="F8" s="1">
-        <v>77.0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>84.0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>88.0</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="E11" s="1">
+        <v>149.0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>160.0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>171.0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>185.0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>199.0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>244.0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>269.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
         <v>95.0</v>
       </c>
-      <c r="J8" s="1">
-        <v>103.0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>110.0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>116.0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>123.0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>140.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>63.0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>77.0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>86.0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>96.0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>104.0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>110.0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>119.0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>127.0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>137.0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>144.0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>154.0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>174.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>50.0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>94.0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>103.0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>117.0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>125.0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>133.0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>145.0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>155.0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>167.0</v>
-      </c>
-      <c r="L10" s="1">
-        <v>175.0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>168.0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>210.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2">
-        <v>100.0</v>
-      </c>
-      <c r="B11" s="1">
-        <v>70.0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>149.0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>160.0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>171.0</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="E12" s="1">
+        <v>180.0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>194.0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>207.0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>241.0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>259.0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>271.0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>296.0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>327.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>208.0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>225.0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>240.0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>250.0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>280.0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>301.0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>314.0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>380.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>150.0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>236.0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>260.0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>278.0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>299.0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>322.0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>343.0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>363.0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>404.0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>438.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
         <v>185.0</v>
       </c>
-      <c r="J11" s="1">
-        <v>199.0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>214.0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>224.0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>244.0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>269.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2">
-        <v>125.0</v>
-      </c>
-      <c r="B12" s="1">
-        <v>95.0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>180.0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>194.0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>207.0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>224.0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>241.0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>259.0</v>
-      </c>
-      <c r="L12" s="1">
-        <v>271.0</v>
-      </c>
-      <c r="M12" s="1">
-        <v>296.0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>327.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2">
-        <v>160.0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>208.0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>225.0</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="E15" s="1">
+        <v>268.0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>297.0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>317.0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>341.0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>368.0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>391.0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>415.0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>464.0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>500.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
         <v>240.0</v>
       </c>
-      <c r="I13" s="1">
-        <v>250.0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>280.0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>301.0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>314.0</v>
-      </c>
-      <c r="M13" s="1">
-        <v>348.0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>380.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2">
-        <v>200.0</v>
-      </c>
-      <c r="B14" s="1">
-        <v>150.0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>236.0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>260.0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>278.0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>299.0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>322.0</v>
-      </c>
-      <c r="K14" s="1">
-        <v>343.0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>363.0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>404.0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>438.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2">
-        <v>250.0</v>
-      </c>
-      <c r="B15" s="1">
-        <v>185.0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>268.0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>297.0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>317.0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>341.0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>368.0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>391.0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>415.0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>464.0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="1">
-        <v>240.0</v>
+      <c r="E16" s="1">
+        <v>315.0</v>
       </c>
       <c r="F16" s="1">
-        <v>315.0</v>
+        <v>350.0</v>
       </c>
       <c r="G16" s="1">
-        <v>350.0</v>
+        <v>374.0</v>
       </c>
       <c r="H16" s="1">
-        <v>374.0</v>
+        <v>401.0</v>
       </c>
       <c r="I16" s="1">
-        <v>401.0</v>
+        <v>435.0</v>
       </c>
       <c r="J16" s="1">
-        <v>435.0</v>
+        <v>468.0</v>
       </c>
       <c r="K16" s="1">
-        <v>468.0</v>
+        <v>490.0</v>
       </c>
       <c r="L16" s="1">
-        <v>490.0</v>
+        <v>552.0</v>
       </c>
       <c r="M16" s="1">
-        <v>552.0</v>
-      </c>
-      <c r="N16" s="1">
         <v>590.0</v>
       </c>
     </row>
@@ -1932,6 +1892,96 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>63.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>250.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>

</xml_diff>